<commit_message>
add data preprocessing scripts
</commit_message>
<xml_diff>
--- a/study_files/all_participants.xlsx
+++ b/study_files/all_participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ee21308d1ee2822/My_GitHub_Repos/HRI/study_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="764" documentId="11_F25DC773A252ABDACC1048B919D96BBE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE89FE73-4521-4495-8DAD-0CF5C6E6FB62}"/>
+  <xr:revisionPtr revIDLastSave="949" documentId="11_F25DC773A252ABDACC1048B919D96BBE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDF55446-0AF3-4E5A-B8F3-ED099682FB78}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -152,97 +152,163 @@
     <t>+61 413 396 153</t>
   </si>
   <si>
+    <t>dannypoonau@gmail.com</t>
+  </si>
+  <si>
+    <t>+61 438 021 371</t>
+  </si>
+  <si>
+    <t>viyagulav@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 469 787 934</t>
+  </si>
+  <si>
+    <t>xueyangk@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 461 571 827</t>
+  </si>
+  <si>
+    <t>Tung Khanh Ho (M)</t>
+  </si>
+  <si>
+    <t>Eddie Zhao (M?)</t>
+  </si>
+  <si>
+    <t>Jialin Huang (M?)</t>
+  </si>
+  <si>
+    <t>Qi Sun (M)</t>
+  </si>
+  <si>
+    <t>Aksay Kashyap (M)</t>
+  </si>
+  <si>
+    <t>Danny Poon (M)</t>
+  </si>
+  <si>
+    <t>Viyagula Varsha Vedaraj (F)</t>
+  </si>
+  <si>
+    <t>Alex Kang (M)</t>
+  </si>
+  <si>
+    <t>chungnanh@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 481 958 626</t>
+  </si>
+  <si>
+    <t>Chung-Nan Hsiao (M)</t>
+  </si>
+  <si>
+    <t>mwongsodirdj@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 412 723 582</t>
+  </si>
+  <si>
+    <t>Matthew Wongsodirdjo (M)</t>
+  </si>
+  <si>
+    <t>majain@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 431 800 116</t>
+  </si>
+  <si>
+    <t>Mayank Jain (M)</t>
+  </si>
+  <si>
+    <t>Weijian Chen (M)</t>
+  </si>
+  <si>
+    <t>weijianc@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 404 153 521</t>
+  </si>
+  <si>
+    <t>Fadil Fahri (M)</t>
+  </si>
+  <si>
+    <t>fahrif@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 481 752 181</t>
+  </si>
+  <si>
+    <t>Siri He (F)</t>
+  </si>
+  <si>
+    <t>Binh Tran (M)</t>
+  </si>
+  <si>
+    <t>Yongqing Chen (F)</t>
+  </si>
+  <si>
+    <t>yongqingc1@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 423 597 827</t>
+  </si>
+  <si>
+    <t>Olivia Santoso (F)</t>
+  </si>
+  <si>
+    <t>osantoso@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 422 528 011</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Bavatharani Maheswaran (F)</t>
+  </si>
+  <si>
+    <t>bmaheswaran99@gmail.com</t>
+  </si>
+  <si>
+    <t>+61 450 874 933</t>
+  </si>
+  <si>
+    <t>Wangpeng Gui (M)</t>
+  </si>
+  <si>
     <t>wgui@student.unimelb.edu.au</t>
   </si>
   <si>
     <t>+61 466 624 169</t>
   </si>
   <si>
-    <t>dannypoonau@gmail.com</t>
-  </si>
-  <si>
-    <t>+61 438 021 371</t>
-  </si>
-  <si>
-    <t>viyagulav@student.unimelb.edu.au</t>
-  </si>
-  <si>
-    <t>+61 469 787 934</t>
-  </si>
-  <si>
-    <t>sahoon@student.unimelb.edu.au</t>
-  </si>
-  <si>
-    <t>+61 421 200 030</t>
-  </si>
-  <si>
-    <t>xueyangk@student.unimelb.edu.au</t>
-  </si>
-  <si>
-    <t>+61 461 571 827</t>
-  </si>
-  <si>
-    <t>Tung Khanh Ho (M)</t>
-  </si>
-  <si>
-    <t>Eddie Zhao (M?)</t>
-  </si>
-  <si>
-    <t>Siri He (M?)</t>
-  </si>
-  <si>
-    <t>Jialin Huang (M?)</t>
-  </si>
-  <si>
-    <t>Qi Sun (M)</t>
-  </si>
-  <si>
-    <t>Binh Tran (M?)</t>
-  </si>
-  <si>
-    <t>Aksay Kashyap (M)</t>
-  </si>
-  <si>
-    <t>Wangpeng Gui (M)</t>
-  </si>
-  <si>
-    <t>Danny Poon (M)</t>
-  </si>
-  <si>
-    <t>Viyagula Varsha Vedaraj (F)</t>
-  </si>
-  <si>
-    <t>Nishant Sahoo (M)</t>
-  </si>
-  <si>
-    <t>Alex Kang (M)</t>
-  </si>
-  <si>
-    <t>chungnanh@student.unimelb.edu.au</t>
-  </si>
-  <si>
-    <t>+61 481 958 626</t>
-  </si>
-  <si>
-    <t>Chung-Nan Hsiao (M)</t>
-  </si>
-  <si>
-    <t>mwongsodirdj@student.unimelb.edu.au</t>
-  </si>
-  <si>
-    <t>+61 412 723 582</t>
-  </si>
-  <si>
-    <t>Matthew Wongsodirdjo (M)</t>
-  </si>
-  <si>
-    <t>majain@student.unimelb.edu.au</t>
-  </si>
-  <si>
-    <t>+61 431 800 116</t>
-  </si>
-  <si>
-    <t>Mayank Jain (M)</t>
+    <t>Le Fang (M)</t>
+  </si>
+  <si>
+    <t>fredfang1203@gmail.com</t>
+  </si>
+  <si>
+    <t>+61 433 763 252</t>
+  </si>
+  <si>
+    <t>okayolya03@gmail.com</t>
+  </si>
+  <si>
+    <t>+61 478 607 096</t>
+  </si>
+  <si>
+    <t>Olya Serova (F)</t>
+  </si>
+  <si>
+    <t>dotooaddo@student.unimelb.edu.au</t>
+  </si>
+  <si>
+    <t>+61 435 153 698</t>
+  </si>
+  <si>
+    <t>Derrick Kelvin Otoo-Addo (M)</t>
   </si>
 </sst>
 </file>
@@ -598,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -658,14 +724,19 @@
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="F2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -676,7 +747,12 @@
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="F3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
@@ -693,37 +769,70 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="F5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="F6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="F7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -739,15 +848,7 @@
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C9" s="4"/>
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
@@ -757,15 +858,7 @@
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="C10" s="4"/>
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
@@ -775,10 +868,24 @@
       <c r="A11" s="1">
         <v>8</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="F11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
@@ -795,7 +902,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>34</v>
@@ -806,16 +913,35 @@
       <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="F13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="F14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -841,42 +967,51 @@
       <c r="A17" s="1">
         <v>12</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="F17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>14</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>10</v>
@@ -898,13 +1033,13 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>15</v>
@@ -916,7 +1051,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>30</v>
@@ -945,13 +1080,13 @@
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
@@ -1000,13 +1135,13 @@
         <v>21</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>19</v>
@@ -1019,7 +1154,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>26</v>
@@ -1049,6 +1184,15 @@
       <c r="A32" s="1">
         <v>23</v>
       </c>
+      <c r="B32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>20</v>
       </c>
@@ -1060,7 +1204,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>36</v>
@@ -1076,6 +1220,15 @@
     <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>25</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>13</v>
@@ -1105,6 +1258,15 @@
       <c r="A37" s="1">
         <v>27</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>23</v>
       </c>
@@ -1116,13 +1278,13 @@
         <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>10</v>
@@ -1139,67 +1301,147 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>29</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>30</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="3"/>
+    </row>
     <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="1">
-        <f>COUNTA(B2:B38)</f>
-        <v>15</v>
-      </c>
-      <c r="G43" s="1">
-        <f>COUNTA(G2:G38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+      <c r="A43" s="1">
+        <v>31</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>32</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="3"/>
+    </row>
     <row r="45" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>33</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="3"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+    </row>
     <row r="47" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B50" s="1">
+        <f>COUNTA(B2:B45)</f>
+        <v>22</v>
+      </c>
+      <c r="G50" s="1">
+        <f>COUNTA(G2:G45)</f>
+        <v>10</v>
+      </c>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="I53" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="mailto:xinruihe42@gmail.com" xr:uid="{43679BA1-D1ED-4DC9-84CF-8FECE2FAF3F4}"/>
     <hyperlink ref="C30" r:id="rId2" display="mailto:yuhzhao3@student.unimelb.edu.au" xr:uid="{6AE5A759-0C60-45B5-90DD-8B38282B24DB}"/>
-    <hyperlink ref="C21" r:id="rId3" display="mailto:jialin.huang3@student.unimelb.edu.au" xr:uid="{59A0EDE9-6C43-40E4-B22A-0FA0C5859323}"/>
+    <hyperlink ref="C34" r:id="rId3" display="mailto:jialin.huang3@student.unimelb.edu.au" xr:uid="{59A0EDE9-6C43-40E4-B22A-0FA0C5859323}"/>
     <hyperlink ref="C22" r:id="rId4" display="mailto:sunqs@student.unimelb.edu.au" xr:uid="{BFA6AC8F-8142-4D22-A149-5F777BC5152E}"/>
     <hyperlink ref="C3" r:id="rId5" display="mailto:tranbinhofficial@gmail.com" xr:uid="{3A4EE697-18FA-4BA7-A956-AE1DB9ECCF02}"/>
     <hyperlink ref="C13" r:id="rId6" display="mailto:akshay.kashyap@student.unimelb.edu.au" xr:uid="{47E4EE04-3920-48D3-B1D0-539583F0EB30}"/>
     <hyperlink ref="C33" r:id="rId7" display="mailto:tungkhanhh@student.unimelb.edu.au" xr:uid="{FC47B24D-AE6B-4ED1-B34E-714E473CE9E3}"/>
-    <hyperlink ref="C9" r:id="rId8" display="mailto:wgui@student.unimelb.edu.au" xr:uid="{8AB4D7C4-B2AD-4694-8226-959EB6143D7F}"/>
-    <hyperlink ref="C5" r:id="rId9" display="mailto:dannypoonau@gmail.com" xr:uid="{06C559E7-CBE8-4335-9C94-652D30490F7C}"/>
-    <hyperlink ref="C18" r:id="rId10" display="mailto:viyagulav@student.unimelb.edu.au" xr:uid="{75FB2DE0-32BC-4A60-9820-6E359D2EE758}"/>
-    <hyperlink ref="C10" r:id="rId11" display="mailto:sahoon@student.unimelb.edu.au" xr:uid="{EBA564C4-7F82-4D1F-B6EE-C14D0B416AD1}"/>
-    <hyperlink ref="C19" r:id="rId12" display="mailto:xueyangk@student.unimelb.edu.au" xr:uid="{484570F8-50AE-4304-A602-0FD27DC28218}"/>
-    <hyperlink ref="C24" r:id="rId13" xr:uid="{92C7837C-B21A-4FE2-83F8-D5988225A373}"/>
-    <hyperlink ref="C29" r:id="rId14" display="mailto:mwongsodirdj@student.unimelb.edu.au" xr:uid="{9425F88E-CBC1-46A6-90A1-F68443ECE712}"/>
-    <hyperlink ref="C38" r:id="rId15" display="mailto:majain@student.unimelb.edu.au" xr:uid="{FE814408-19BA-4E66-8CC3-AE2599F5B0E9}"/>
+    <hyperlink ref="C5" r:id="rId8" display="mailto:dannypoonau@gmail.com" xr:uid="{06C559E7-CBE8-4335-9C94-652D30490F7C}"/>
+    <hyperlink ref="C18" r:id="rId9" display="mailto:viyagulav@student.unimelb.edu.au" xr:uid="{75FB2DE0-32BC-4A60-9820-6E359D2EE758}"/>
+    <hyperlink ref="C11" r:id="rId10" display="mailto:xueyangk@student.unimelb.edu.au" xr:uid="{484570F8-50AE-4304-A602-0FD27DC28218}"/>
+    <hyperlink ref="C24" r:id="rId11" xr:uid="{92C7837C-B21A-4FE2-83F8-D5988225A373}"/>
+    <hyperlink ref="C29" r:id="rId12" display="mailto:mwongsodirdj@student.unimelb.edu.au" xr:uid="{9425F88E-CBC1-46A6-90A1-F68443ECE712}"/>
+    <hyperlink ref="C38" r:id="rId13" display="mailto:majain@student.unimelb.edu.au" xr:uid="{FE814408-19BA-4E66-8CC3-AE2599F5B0E9}"/>
+    <hyperlink ref="C6" r:id="rId14" display="mailto:weijianc@student.unimelb.edu.au" xr:uid="{5559A620-BCA1-43F5-830C-40FCFCA79290}"/>
+    <hyperlink ref="C7" r:id="rId15" display="mailto:fahrif@student.unimelb.edu.au" xr:uid="{86ED7B45-F17C-47B5-8EB5-8EF6574E8AAA}"/>
+    <hyperlink ref="C14" r:id="rId16" display="mailto:yongqingc1@student.unimelb.edu.au" xr:uid="{B50E7D43-7EDC-433F-A8DD-A6BFF07CDB52}"/>
+    <hyperlink ref="C40" r:id="rId17" display="mailto:osantoso@student.unimelb.edu.au" xr:uid="{2CD1191D-6274-460D-95E5-DA1B1217F244}"/>
+    <hyperlink ref="C21" r:id="rId18" xr:uid="{721E6044-EBA5-4F6C-97B2-0831A82383BB}"/>
+    <hyperlink ref="C17" r:id="rId19" display="mailto:wgui@student.unimelb.edu.au" xr:uid="{BAF0ADE2-5778-44C5-A9AB-3A46D563D2FB}"/>
+    <hyperlink ref="C37" r:id="rId20" display="mailto:fredfang1203@gmail.com" xr:uid="{3F93C12B-8345-4EAC-A604-2CADC435A484}"/>
+    <hyperlink ref="C32" r:id="rId21" display="mailto:okayolya03@gmail.com" xr:uid="{4AD0418E-9A03-4137-8D5C-5D1B39707556}"/>
+    <hyperlink ref="C45" r:id="rId22" display="mailto:dotooaddo@student.unimelb.edu.au" xr:uid="{1AF8F291-BA4C-4CDB-A737-E1D48BACA6FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
P22 & P23 cleanup
</commit_message>
<xml_diff>
--- a/study_files/all_participants.xlsx
+++ b/study_files/all_participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ee21308d1ee2822/My_GitHub_Repos/HRI/study_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="995" documentId="11_F25DC773A252ABDACC1048B919D96BBE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38F4C3A1-9081-416D-852A-BAF69179A19B}"/>
+  <xr:revisionPtr revIDLastSave="1025" documentId="11_F25DC773A252ABDACC1048B919D96BBE5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE705037-9D79-4B1D-9A45-9798BFC55DC9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -348,6 +348,21 @@
   </si>
   <si>
     <t>+61 423 518 409</t>
+  </si>
+  <si>
+    <t>Alfred (M) ~4pm</t>
+  </si>
+  <si>
+    <t>wechat</t>
+  </si>
+  <si>
+    <t>Shakiba Barghi (F)</t>
+  </si>
+  <si>
+    <t>shakibabarghi75@gmail.com</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -701,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1251,7 +1266,7 @@
       <c r="G32" s="3"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -1270,9 +1285,12 @@
       <c r="F33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>25</v>
       </c>
@@ -1291,9 +1309,12 @@
       <c r="F34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1302,26 +1323,19 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>26</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="E36" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>27</v>
       </c>
@@ -1337,10 +1351,16 @@
       <c r="E37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G37" s="3"/>
+      <c r="F37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>28</v>
       </c>
@@ -1356,9 +1376,15 @@
       <c r="E38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1367,8 +1393,9 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>29</v>
       </c>
@@ -1384,9 +1411,15 @@
       <c r="E40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>30</v>
       </c>
@@ -1402,9 +1435,13 @@
       <c r="E41" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F41" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1413,8 +1450,9 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>31</v>
       </c>
@@ -1431,26 +1469,28 @@
         <v>16</v>
       </c>
       <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>32</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>33</v>
       </c>
@@ -1468,8 +1508,9 @@
       </c>
       <c r="G45" s="3"/>
       <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1478,62 +1519,109 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B49" s="2" t="s">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>35</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J49" s="1"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B50" s="1">
-        <f>COUNTA(B2:B45)</f>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B52" s="1">
+        <f>COUNTA(B2:B48)</f>
         <v>25</v>
       </c>
-      <c r="G50" s="1">
-        <f>COUNTA(G2:G45)</f>
-        <v>15</v>
-      </c>
-      <c r="J50" s="1"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G52" s="1">
+        <f>COUNTA(G2:G48)</f>
+        <v>20</v>
+      </c>
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B53" s="1" t="s">
+      <c r="I53" s="2"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B55" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B54" s="1" t="s">
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B56" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B57" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="mailto:xinruihe42@gmail.com" xr:uid="{43679BA1-D1ED-4DC9-84CF-8FECE2FAF3F4}"/>
-    <hyperlink ref="C53" r:id="rId2" display="mailto:yuhzhao3@student.unimelb.edu.au" xr:uid="{6AE5A759-0C60-45B5-90DD-8B38282B24DB}"/>
+    <hyperlink ref="C55" r:id="rId2" display="mailto:yuhzhao3@student.unimelb.edu.au" xr:uid="{6AE5A759-0C60-45B5-90DD-8B38282B24DB}"/>
     <hyperlink ref="C34" r:id="rId3" display="mailto:jialin.huang3@student.unimelb.edu.au" xr:uid="{59A0EDE9-6C43-40E4-B22A-0FA0C5859323}"/>
     <hyperlink ref="C22" r:id="rId4" display="mailto:sunqs@student.unimelb.edu.au" xr:uid="{BFA6AC8F-8142-4D22-A149-5F777BC5152E}"/>
     <hyperlink ref="C3" r:id="rId5" display="mailto:tranbinhofficial@gmail.com" xr:uid="{3A4EE697-18FA-4BA7-A956-AE1DB9ECCF02}"/>
@@ -1549,12 +1637,12 @@
     <hyperlink ref="C7" r:id="rId15" display="mailto:fahrif@student.unimelb.edu.au" xr:uid="{86ED7B45-F17C-47B5-8EB5-8EF6574E8AAA}"/>
     <hyperlink ref="C14" r:id="rId16" display="mailto:yongqingc1@student.unimelb.edu.au" xr:uid="{B50E7D43-7EDC-433F-A8DD-A6BFF07CDB52}"/>
     <hyperlink ref="C40" r:id="rId17" display="mailto:osantoso@student.unimelb.edu.au" xr:uid="{2CD1191D-6274-460D-95E5-DA1B1217F244}"/>
-    <hyperlink ref="C36" r:id="rId18" xr:uid="{721E6044-EBA5-4F6C-97B2-0831A82383BB}"/>
+    <hyperlink ref="C57" r:id="rId18" xr:uid="{721E6044-EBA5-4F6C-97B2-0831A82383BB}"/>
     <hyperlink ref="C17" r:id="rId19" display="mailto:wgui@student.unimelb.edu.au" xr:uid="{BAF0ADE2-5778-44C5-A9AB-3A46D563D2FB}"/>
     <hyperlink ref="C37" r:id="rId20" display="mailto:fredfang1203@gmail.com" xr:uid="{3F93C12B-8345-4EAC-A604-2CADC435A484}"/>
-    <hyperlink ref="C54" r:id="rId21" display="mailto:okayolya03@gmail.com" xr:uid="{4AD0418E-9A03-4137-8D5C-5D1B39707556}"/>
+    <hyperlink ref="C56" r:id="rId21" display="mailto:okayolya03@gmail.com" xr:uid="{4AD0418E-9A03-4137-8D5C-5D1B39707556}"/>
     <hyperlink ref="C45" r:id="rId22" display="mailto:dotooaddo@student.unimelb.edu.au" xr:uid="{1AF8F291-BA4C-4CDB-A737-E1D48BACA6FB}"/>
-    <hyperlink ref="C44" r:id="rId23" display="mailto:jamesandersonwriting@gmail.com" xr:uid="{2A391F19-3AE9-484F-A2A1-25E277568AA6}"/>
+    <hyperlink ref="C58" r:id="rId23" display="mailto:jamesandersonwriting@gmail.com" xr:uid="{2A391F19-3AE9-484F-A2A1-25E277568AA6}"/>
     <hyperlink ref="C41" r:id="rId24" display="mailto:phartanti@student.unimelb.edu.au" xr:uid="{86142654-F463-4A41-AF49-95257D4C1C92}"/>
     <hyperlink ref="C28" r:id="rId25" display="mailto:tianyingw2@student.unimleb.edu.au" xr:uid="{D33E86D1-403C-48F6-9BA6-831477D5339F}"/>
     <hyperlink ref="C21" r:id="rId26" xr:uid="{0F1AB21C-8D6B-4E45-8D7A-7051B0C9ACA2}"/>

</xml_diff>